<commit_message>
QCADOOCLS-6844 Renamed package, fixed problem with date parsers, added additional validations to positions import.
</commit_message>
<xml_diff>
--- a/mes-plugins/mes-plugins-material-flow-resources/src/main/resources/materialFlowResources/public/resources/positionImportSchema_pl.xlsx
+++ b/mes-plugins/mes-plugins-material-flow-resources/src/main/resources/materialFlowResources/public/resources/positionImportSchema_pl.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lupo/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lupo/qcadoo-src/mes/mes-plugins/mes-plugins-material-flow-resources/src/main/resources/materialFlowResources/public/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B39CF7C-8F0B-9541-9D58-AD8FB9917D19}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1686822C-5182-724B-83C3-C73D7DA11530}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16760" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -400,7 +400,7 @@
   <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -432,10 +432,10 @@
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>7</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>8</v>

</xml_diff>